<commit_message>
Tables 1 and 2 up
</commit_message>
<xml_diff>
--- a/C15H/A4_C15_H_good.xlsx
+++ b/C15H/A4_C15_H_good.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Windows\ServiceProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_3227\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="87" documentId="8_{AC782490-6839-4A74-A9DF-C6C67A99C109}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{CC69DD8E-9513-4D35-9FF5-2E617EB2757E}"/>
+  <xr:revisionPtr revIDLastSave="96" documentId="8_{AC782490-6839-4A74-A9DF-C6C67A99C109}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{9C8F4CB8-7D99-4C56-AF41-855EDD3C3AC0}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7052,8 +7052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AEAFB21-CB9D-4705-9E61-FE1D9FF66C74}">
   <dimension ref="A1:K1981"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="125" zoomScaleSheetLayoutView="100" workbookViewId="0" xr3:uid="{F74D3B2B-70BC-5F5E-8098-66CE1AE9E490}">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="A1405" zoomScaleNormal="125" zoomScaleSheetLayoutView="100" workbookViewId="0" xr3:uid="{F74D3B2B-70BC-5F5E-8098-66CE1AE9E490}">
+      <selection activeCell="I1433" sqref="I1433"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.15"/>
@@ -19563,7 +19563,7 @@
         <v>5.4563834131003066</v>
       </c>
       <c r="I321" s="4">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="J321" s="4">
         <v>0.56430664062500002</v>
@@ -23853,7 +23853,7 @@
         <v>20.828401745752029</v>
       </c>
       <c r="I431" s="4">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="J431" s="4">
         <v>3.5160644531250003</v>
@@ -28143,7 +28143,7 @@
         <v>20.735375815208471</v>
       </c>
       <c r="I541" s="4">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="J541" s="4">
         <v>3.8633300781250002</v>
@@ -32433,7 +32433,7 @@
         <v>20.40644575623433</v>
       </c>
       <c r="I651" s="4">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="J651" s="4">
         <v>12.979052734375001</v>
@@ -36723,7 +36723,7 @@
         <v>5.4563834131003066</v>
       </c>
       <c r="I761" s="4">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="J761" s="4">
         <v>0.651123046875</v>
@@ -41013,7 +41013,7 @@
         <v>5.2762548657640922</v>
       </c>
       <c r="I871" s="4">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="J871" s="4">
         <v>0.52089843750000009</v>
@@ -49593,7 +49593,7 @@
         <v>24.536003432890116</v>
       </c>
       <c r="I1091" s="4">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="J1091" s="4">
         <v>4.4276367187500005</v>
@@ -53883,7 +53883,7 @@
         <v>25.158448623373143</v>
       </c>
       <c r="I1201" s="4">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="J1201" s="4">
         <v>5.9903320312500004</v>
@@ -58173,7 +58173,7 @@
         <v>25.042918629986705</v>
       </c>
       <c r="I1311" s="4">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="J1311" s="4">
         <v>6.0337402343750002</v>

</xml_diff>